<commit_message>
Updated Datastructure for raw data and all the other things like bugfixes and try-expect statements
</commit_message>
<xml_diff>
--- a/API_Calls/currency-codes.xlsx
+++ b/API_Calls/currency-codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asasc\Documents\Python Scripts\DHBW\API_Thing\API_Calls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A12BF18-CE00-4CC7-9ADD-7E0199A3064C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8609C6-1449-4E82-9845-4832EE57C13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28935" yWindow="2625" windowWidth="28110" windowHeight="15885" xr2:uid="{7D1FEA51-8815-0448-9B98-8FEB207BCDBB}"/>
+    <workbookView xWindow="4755" yWindow="3255" windowWidth="28110" windowHeight="15885" xr2:uid="{7D1FEA51-8815-0448-9B98-8FEB207BCDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1704,9 +1704,6 @@
     <t xml:space="preserve">VEREINIGTE STAATEN VON AMERIKA </t>
   </si>
   <si>
-    <t>VEREINIGTE STAATEN VON AMERIKA</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
@@ -1837,6 +1834,9 @@
   </si>
   <si>
     <t>COTE D'IVOIRE</t>
+  </si>
+  <si>
+    <t>VEREINIGTE STAATEN</t>
   </si>
 </sst>
 </file>
@@ -2190,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B3565-D280-2E40-8385-C5AE1329A397}">
   <dimension ref="A1:D277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="F248" sqref="F248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2302,7 +2302,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
         <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C43" t="s">
         <v>107</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
@@ -2881,10 +2881,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>567</v>
+      </c>
+      <c r="B50" t="s">
         <v>568</v>
-      </c>
-      <c r="B50" t="s">
-        <v>569</v>
       </c>
       <c r="C50" t="s">
         <v>117</v>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B62" t="s">
         <v>133</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
@@ -3077,10 +3077,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B64" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C64" t="s">
         <v>117</v>
@@ -3189,10 +3189,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B72" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C72" t="s">
         <v>117</v>
@@ -3413,7 +3413,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B88" t="s">
         <v>181</v>
@@ -3472,7 +3472,7 @@
         <v>189</v>
       </c>
       <c r="B92" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C92" t="s">
         <v>190</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B100" t="s">
         <v>10</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B171" t="s">
         <v>10</v>
@@ -4631,10 +4631,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B175" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4779,10 +4779,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>574</v>
+      </c>
+      <c r="B186" t="s">
         <v>575</v>
-      </c>
-      <c r="B186" t="s">
-        <v>576</v>
       </c>
       <c r="C186" t="s">
         <v>370</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B189" t="s">
         <v>13</v>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B190" t="s">
         <v>13</v>
@@ -5076,7 +5076,7 @@
         <v>544</v>
       </c>
       <c r="B207" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C207" t="s">
         <v>107</v>
@@ -5325,10 +5325,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>593</v>
+      </c>
+      <c r="B225" t="s">
         <v>594</v>
-      </c>
-      <c r="B225" t="s">
-        <v>595</v>
       </c>
       <c r="C225" t="s">
         <v>446</v>
@@ -5339,7 +5339,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B226" t="s">
         <v>257</v>
@@ -5353,10 +5353,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B227" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5571,10 +5571,10 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
+        <v>597</v>
+      </c>
+      <c r="B243" t="s">
         <v>598</v>
-      </c>
-      <c r="B243" t="s">
-        <v>599</v>
       </c>
       <c r="C243" t="s">
         <v>476</v>
@@ -5739,7 +5739,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B255" t="s">
         <v>10</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B256" t="s">
         <v>10</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>556</v>
+        <v>600</v>
       </c>
       <c r="B257" t="s">
         <v>10</v>
@@ -5784,7 +5784,7 @@
         <v>555</v>
       </c>
       <c r="B258" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C258" t="s">
         <v>502</v>
@@ -5795,7 +5795,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B259" t="s">
         <v>158</v>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B260" t="s">
         <v>158</v>
@@ -5823,7 +5823,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B261" t="s">
         <v>158</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B262" t="s">
         <v>158</v>
@@ -5851,7 +5851,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B263" t="s">
         <v>158</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B264" t="s">
         <v>158</v>
@@ -5879,7 +5879,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B265" t="s">
         <v>503</v>
@@ -5963,7 +5963,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B271" t="s">
         <v>136</v>
@@ -5991,10 +5991,10 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>577</v>
+      </c>
+      <c r="B273" t="s">
         <v>578</v>
-      </c>
-      <c r="B273" t="s">
-        <v>579</v>
       </c>
       <c r="C273" t="s">
         <v>515</v>
@@ -6005,7 +6005,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B274" t="s">
         <v>136</v>
@@ -6019,10 +6019,10 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>580</v>
+      </c>
+      <c r="B275" t="s">
         <v>581</v>
-      </c>
-      <c r="B275" t="s">
-        <v>582</v>
       </c>
       <c r="C275" t="s">
         <v>516</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B276" t="s">
         <v>13</v>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B277" t="s">
         <v>13</v>

</xml_diff>